<commit_message>
Feature #1003 :: Client Operations - Télécharger un échantillon
</commit_message>
<xml_diff>
--- a/src/Application/Sonata/ClientOperationsBundle/Resources/public/excel/blank.xlsx
+++ b/src/Application/Sonata/ClientOperationsBundle/Resources/public/excel/blank.xlsx
@@ -1711,7 +1711,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2026,33 +2026,33 @@
       <c r="E8" s="88"/>
       <c r="F8" s="33"/>
       <c r="G8" s="151">
-        <f t="shared" ref="G3:G40" si="7">F8*E8</f>
+        <f t="shared" ref="G8:G40" si="7">F8*E8</f>
         <v>0</v>
       </c>
       <c r="H8" s="151">
-        <f t="shared" ref="H3:H40" si="8">+G8+E8</f>
+        <f t="shared" ref="H8:H40" si="8">+G8+E8</f>
         <v>0</v>
       </c>
       <c r="I8" s="151">
-        <f t="shared" ref="I3:I40" si="9">H8</f>
+        <f t="shared" ref="I8:I40" si="9">H8</f>
         <v>0</v>
       </c>
       <c r="J8" s="152">
-        <f t="shared" ref="J3:J40" si="10">D8</f>
+        <f t="shared" ref="J8:J40" si="10">D8</f>
         <v>0</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="146" t="str">
-        <f t="shared" ref="L3:L40" si="11">IF(K8&lt;&gt;"",K8,"")</f>
+        <f t="shared" ref="L8:L40" si="11">IF(K8&lt;&gt;"",K8,"")</f>
         <v/>
       </c>
       <c r="M8" s="35"/>
       <c r="N8" s="151">
-        <f t="shared" ref="N3:N40" si="12">IF(M8&lt;&gt;"",E8/M8,)</f>
+        <f t="shared" ref="N8:N40" si="12">IF(M8&lt;&gt;"",E8/M8,)</f>
         <v>0</v>
       </c>
       <c r="O8" s="151">
-        <f t="shared" ref="O3:O40" si="13">N8*F8</f>
+        <f t="shared" ref="O8:O40" si="13">N8*F8</f>
         <v>0</v>
       </c>
       <c r="P8" s="36"/>
@@ -3456,7 +3456,7 @@
     <sheetView showZeros="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3755,17 +3755,17 @@
       <c r="E6" s="88"/>
       <c r="F6" s="88"/>
       <c r="G6" s="117" t="str">
-        <f t="shared" ref="G4:G40" si="6">IF(B6&lt;&gt;"",B6,"")</f>
+        <f t="shared" ref="G6:G40" si="6">IF(B6&lt;&gt;"",B6,"")</f>
         <v/>
       </c>
       <c r="H6" s="96"/>
       <c r="I6" s="107"/>
       <c r="J6" s="118">
-        <f t="shared" ref="J3:J39" si="7">IF(H6&lt;&gt;"",E6/H6,)</f>
+        <f t="shared" ref="J6:J39" si="7">IF(H6&lt;&gt;"",E6/H6,)</f>
         <v>0</v>
       </c>
       <c r="K6" s="118">
-        <f t="shared" ref="K3:K40" si="8">F6*J6</f>
+        <f t="shared" ref="K6:K40" si="8">F6*J6</f>
         <v>0</v>
       </c>
       <c r="L6" s="109"/>
@@ -3774,15 +3774,15 @@
       <c r="O6" s="56"/>
       <c r="P6" s="56"/>
       <c r="Q6" s="141">
-        <f t="shared" ref="Q3:Q40" si="9">IF(AND(L6="OUI",I6&lt;&gt;19,I6&lt;&gt;""),E6/H6,)</f>
+        <f t="shared" ref="Q6:Q40" si="9">IF(AND(L6="OUI",I6&lt;&gt;19,I6&lt;&gt;""),E6/H6,)</f>
         <v>0</v>
       </c>
       <c r="R6" s="121">
-        <f t="shared" ref="R3:R40" si="10">I6</f>
+        <f t="shared" ref="R6:R40" si="10">I6</f>
         <v>0</v>
       </c>
       <c r="S6" s="141">
-        <f t="shared" ref="S2:S40" si="11">IF(AND(L6="OUI",G6&lt;&gt;""),E6/H6,)</f>
+        <f t="shared" ref="S6:S40" si="11">IF(AND(L6="OUI",G6&lt;&gt;""),E6/H6,)</f>
         <v>0</v>
       </c>
       <c r="T6" s="56"/>
@@ -5523,7 +5523,7 @@
   <dimension ref="A1:IU43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -6821,7 +6821,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -7424,7 +7424,7 @@
     <sheetView showZeros="0" tabSelected="1" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -7968,7 +7968,7 @@
     <sheetView showZeros="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -8206,12 +8206,12 @@
       <c r="E12" s="32"/>
       <c r="F12" s="85"/>
       <c r="G12" s="146" t="str">
-        <f t="shared" ref="G3:G40" si="2">IF(C12&lt;&gt;"",C12,"")</f>
+        <f t="shared" ref="G12:G40" si="2">IF(C12&lt;&gt;"",C12,"")</f>
         <v/>
       </c>
       <c r="H12" s="35"/>
       <c r="I12" s="147">
-        <f t="shared" ref="I3:I40" si="3">IF(H12&lt;&gt;"",F12/H12,)</f>
+        <f t="shared" ref="I12:I40" si="3">IF(H12&lt;&gt;"",F12/H12,)</f>
         <v>0</v>
       </c>
       <c r="J12" s="115"/>
@@ -9729,12 +9729,12 @@
       <c r="E19" s="56"/>
       <c r="F19" s="88"/>
       <c r="G19" s="146" t="str">
-        <f t="shared" ref="G3:G40" si="6">IF(C19&lt;&gt;"",C19,"")</f>
+        <f t="shared" ref="G19:G40" si="6">IF(C19&lt;&gt;"",C19,"")</f>
         <v/>
       </c>
       <c r="H19" s="96"/>
       <c r="I19" s="147">
-        <f t="shared" ref="I3:I40" si="7">IF(H19&lt;&gt;"",F19/H19,)</f>
+        <f t="shared" ref="I19:I40" si="7">IF(H19&lt;&gt;"",F19/H19,)</f>
         <v>0</v>
       </c>
       <c r="J19" s="107"/>
@@ -9744,15 +9744,15 @@
       <c r="N19" s="56"/>
       <c r="O19" s="56"/>
       <c r="P19" s="149">
-        <f t="shared" ref="P3:P40" si="8">IF(AND(K19="OUI",J19&lt;&gt;"",OR(J19&lt;29,J19=31)),F19/H19,)</f>
+        <f t="shared" ref="P19:P40" si="8">IF(AND(K19="OUI",J19&lt;&gt;"",OR(J19&lt;29,J19=31)),F19/H19,)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="150">
-        <f t="shared" ref="Q3:Q40" si="9">J19</f>
+        <f t="shared" ref="Q19:Q40" si="9">J19</f>
         <v>0</v>
       </c>
       <c r="R19" s="149">
-        <f t="shared" ref="R3:R40" si="10">I19</f>
+        <f t="shared" ref="R19:R40" si="10">I19</f>
         <v>0</v>
       </c>
       <c r="S19" s="56"/>
@@ -9763,7 +9763,7 @@
       <c r="X19" s="56"/>
       <c r="Y19" s="56"/>
       <c r="Z19" s="125">
-        <f t="shared" ref="Z3:Z40" si="11">IF(J19&lt;&gt;29,B19,)</f>
+        <f t="shared" ref="Z19:Z40" si="11">IF(J19&lt;&gt;29,B19,)</f>
         <v>0</v>
       </c>
     </row>
@@ -10894,7 +10894,7 @@
   <dimension ref="A1:IU43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -12192,7 +12192,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -12347,12 +12347,12 @@
       <c r="D8" s="32"/>
       <c r="E8" s="85"/>
       <c r="F8" s="146" t="str">
-        <f t="shared" ref="F5:F40" si="6">IF(B8&lt;&gt;"",B8,"")</f>
+        <f t="shared" ref="F8:F40" si="6">IF(B8&lt;&gt;"",B8,"")</f>
         <v/>
       </c>
       <c r="G8" s="35"/>
       <c r="H8" s="147">
-        <f t="shared" ref="H3:H40" si="7">IF(G8&lt;&gt;"",E8/G8,)</f>
+        <f t="shared" ref="H8:H40" si="7">IF(G8&lt;&gt;"",E8/G8,)</f>
         <v>0</v>
       </c>
       <c r="I8" s="36"/>
@@ -13024,7 +13024,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -13924,7 +13924,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -14753,7 +14753,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -15085,36 +15085,36 @@
       <c r="E8" s="88"/>
       <c r="F8" s="33"/>
       <c r="G8" s="119">
-        <f t="shared" ref="G3:G40" si="8">F8*E8</f>
+        <f t="shared" ref="G8:G40" si="8">F8*E8</f>
         <v>0</v>
       </c>
       <c r="H8" s="119">
-        <f t="shared" ref="H3:H40" si="9">+G8+E8</f>
+        <f t="shared" ref="H8:H40" si="9">+G8+E8</f>
         <v>0</v>
       </c>
       <c r="I8" s="119">
-        <f t="shared" ref="I3:I40" si="10">H8</f>
+        <f t="shared" ref="I8:I40" si="10">H8</f>
         <v>0</v>
       </c>
       <c r="J8" s="120">
-        <f t="shared" ref="J3:J40" si="11">D8</f>
+        <f t="shared" ref="J8:J40" si="11">D8</f>
         <v>0</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="117" t="str">
-        <f t="shared" ref="L3:L40" si="12">IF(K8&lt;&gt;"",K8,"")</f>
+        <f t="shared" ref="L8:L40" si="12">IF(K8&lt;&gt;"",K8,"")</f>
         <v/>
       </c>
       <c r="M8" s="132" t="str">
-        <f t="shared" ref="M3:M40" si="13">IF(D8="euro",1,"")</f>
+        <f t="shared" ref="M8:M40" si="13">IF(D8="euro",1,"")</f>
         <v/>
       </c>
       <c r="N8" s="119">
-        <f t="shared" ref="N3:N40" si="14">IF(M8&lt;&gt;"",E8/M8,)</f>
+        <f t="shared" ref="N8:N40" si="14">IF(M8&lt;&gt;"",E8/M8,)</f>
         <v>0</v>
       </c>
       <c r="O8" s="119">
-        <f t="shared" ref="O3:O40" si="15">N8*F8</f>
+        <f t="shared" ref="O8:O40" si="15">N8*F8</f>
         <v>0</v>
       </c>
       <c r="P8" s="36"/>
@@ -16608,7 +16608,7 @@
     <sheetView showZeros="0" zoomScale="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:K7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -16820,7 +16820,7 @@
       <c r="E8" s="88"/>
       <c r="F8" s="33"/>
       <c r="G8" s="117" t="str">
-        <f t="shared" ref="G3:G40" si="4">IF(B8&lt;&gt;"",B8,"")</f>
+        <f t="shared" ref="G8:G40" si="4">IF(B8&lt;&gt;"",B8,"")</f>
         <v/>
       </c>
       <c r="H8" s="132" t="str">
@@ -16828,11 +16828,11 @@
         <v/>
       </c>
       <c r="I8" s="119">
-        <f t="shared" ref="I4:I40" si="6">IF(H8&lt;&gt;"",E8/H8,)</f>
+        <f t="shared" ref="I8:I40" si="6">IF(H8&lt;&gt;"",E8/H8,)</f>
         <v>0</v>
       </c>
       <c r="J8" s="119">
-        <f t="shared" ref="J4:J40" si="7">I8*F8</f>
+        <f t="shared" ref="J8:J40" si="7">I8*F8</f>
         <v>0</v>
       </c>
       <c r="K8" s="36"/>

</xml_diff>